<commit_message>
chỉnh sửa , add connectionString
</commit_message>
<xml_diff>
--- a/QLKho(database,phancong)/phancongQuanLyKho.xlsx
+++ b/QLKho(database,phancong)/phancongQuanLyKho.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>STT</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Xây dựng module hướng dẫn sử dụng phần mềm (menu Help, F1) chi tiết đến từng chức năng</t>
   </si>
   <si>
-    <t>Xây dựng tài liệu hướng dẫn cài đặt, vận hành</t>
-  </si>
-  <si>
     <t>Ghép nối các module để nhận được phần mềm hoàn chỉnh</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>4.9</t>
   </si>
   <si>
-    <t>4.10</t>
-  </si>
-  <si>
     <t>Thực hiện</t>
   </si>
   <si>
@@ -105,6 +99,9 @@
   </si>
   <si>
     <t>Xây dựng modul quản lý hàng hóa (thêm sửa xóa )</t>
+  </si>
+  <si>
+    <t>Xây dựng modul quản lý Nhà Cung Cấp(thêm , sửa xóa)</t>
   </si>
 </sst>
 </file>
@@ -550,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,77 +576,77 @@
         <v>0</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="5" t="s">
@@ -660,83 +657,82 @@
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>